<commit_message>
Code added for Zip file compressor and is working fine
</commit_message>
<xml_diff>
--- a/Data/(1) TimecardPunch_SK_REG_Paycodes_COMPLETE.xlsx
+++ b/Data/(1) TimecardPunch_SK_REG_Paycodes_COMPLETE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\WFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE9C151-5DBD-407D-9FF7-83AD55C84D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6572BDD3-5ECE-4B80-B658-C76381300F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,10 +489,13 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.75" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>